<commit_message>
update 12 agustus 2025
</commit_message>
<xml_diff>
--- a/Work/MS BRIBox/PM/2/KC Payakumbuh/FORM PM Unit Gadut.xlsx
+++ b/Work/MS BRIBox/PM/2/KC Payakumbuh/FORM PM Unit Gadut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jamil\Work\MS BRIBox\PM\2\KC Payakumbuh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2F9A63-93B7-42BE-ADFB-9AA0BC23784F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3945410E-668D-48BB-AD84-63CED28AE2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Form PM (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form PM'!$A$7:$W$77</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Form PM'!$A$1:$V$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form PM'!$A$7:$W$78</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Form PM'!$A$1:$V$91</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="253">
   <si>
     <t>FORM PM PERANGKAT IT BRIBOX</t>
   </si>
@@ -785,6 +785,21 @@
   </si>
   <si>
     <t>Payakumbuh,  22 Mei 2025</t>
+  </si>
+  <si>
+    <t>MK4Y136236</t>
+  </si>
+  <si>
+    <t>C2-Dot Matrix Printer</t>
+  </si>
+  <si>
+    <t>Epson LQ-2190</t>
+  </si>
+  <si>
+    <t>Z1-C-5499-C2-0001</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1422,6 +1437,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1669,10 +1690,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1704,28 +1725,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="95"/>
-      <c r="S1" s="95"/>
-      <c r="T1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="97"/>
+      <c r="S1" s="97"/>
+      <c r="T1" s="98"/>
     </row>
     <row r="2" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
@@ -1839,10 +1860,10 @@
       <c r="T7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="U7" s="97" t="s">
+      <c r="U7" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="V7" s="98"/>
+      <c r="V7" s="100"/>
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
@@ -2986,10 +3007,10 @@
       <c r="C30" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="D30" s="75" t="s">
+      <c r="D30" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="52" t="s">
+      <c r="E30" s="92" t="s">
         <v>109</v>
       </c>
       <c r="F30" s="72" t="s">
@@ -3022,70 +3043,70 @@
       <c r="W30" s="50"/>
     </row>
     <row r="31" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54">
+      <c r="A31" s="78">
         <v>23</v>
       </c>
-      <c r="B31" s="79" t="s">
+      <c r="B31" s="57" t="s">
+        <v>251</v>
+      </c>
+      <c r="C31" s="80" t="s">
+        <v>248</v>
+      </c>
+      <c r="D31" s="46" t="s">
+        <v>249</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>250</v>
+      </c>
+      <c r="F31" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31" s="80"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="80"/>
+      <c r="M31" s="55"/>
+      <c r="N31" s="55"/>
+      <c r="O31" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="P31" s="80"/>
+      <c r="Q31" s="80"/>
+      <c r="R31" s="80"/>
+      <c r="S31" s="81"/>
+      <c r="T31" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="U31" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="V31" s="80"/>
+      <c r="W31" s="50" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="78">
+        <v>24</v>
+      </c>
+      <c r="B32" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="80" t="s">
+      <c r="C32" s="80" t="s">
         <v>141</v>
       </c>
-      <c r="D31" s="82" t="s">
+      <c r="D32" s="82" t="s">
         <v>142</v>
       </c>
-      <c r="E31" s="80" t="s">
+      <c r="E32" s="80" t="s">
         <v>143</v>
       </c>
-      <c r="F31" s="85" t="s">
+      <c r="F32" s="85" t="s">
         <v>54</v>
-      </c>
-      <c r="G31" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="55"/>
-      <c r="N31" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="O31" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="P31" s="55"/>
-      <c r="Q31" s="55"/>
-      <c r="R31" s="55"/>
-      <c r="S31" s="61"/>
-      <c r="T31" s="80" t="s">
-        <v>95</v>
-      </c>
-      <c r="U31" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="V31" s="55"/>
-      <c r="W31" s="50"/>
-    </row>
-    <row r="32" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54">
-        <v>24</v>
-      </c>
-      <c r="B32" s="57" t="s">
-        <v>244</v>
-      </c>
-      <c r="C32" s="80">
-        <v>8426165</v>
-      </c>
-      <c r="D32" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="80" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" s="85" t="s">
-        <v>94</v>
       </c>
       <c r="G32" s="55" t="s">
         <v>67</v>
@@ -3095,19 +3116,19 @@
       <c r="J32" s="55"/>
       <c r="K32" s="55"/>
       <c r="L32" s="55"/>
-      <c r="M32" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="N32" s="54"/>
-      <c r="O32" s="55"/>
+      <c r="M32" s="55"/>
+      <c r="N32" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="O32" s="55" t="s">
+        <v>67</v>
+      </c>
       <c r="P32" s="55"/>
       <c r="Q32" s="55"/>
-      <c r="R32" s="55" t="s">
-        <v>241</v>
-      </c>
+      <c r="R32" s="55"/>
       <c r="S32" s="61"/>
       <c r="T32" s="80" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="U32" s="55" t="s">
         <v>67</v>
@@ -3116,14 +3137,14 @@
       <c r="W32" s="50"/>
     </row>
     <row r="33" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54">
+      <c r="A33" s="78">
         <v>25</v>
       </c>
       <c r="B33" s="57" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C33" s="80">
-        <v>8426176</v>
+        <v>8426165</v>
       </c>
       <c r="D33" s="46" t="s">
         <v>65</v>
@@ -3146,11 +3167,13 @@
         <v>67</v>
       </c>
       <c r="N33" s="54"/>
-      <c r="O33" s="55"/>
+      <c r="O33" s="55" t="s">
+        <v>67</v>
+      </c>
       <c r="P33" s="55"/>
       <c r="Q33" s="55"/>
       <c r="R33" s="55" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="S33" s="61"/>
       <c r="T33" s="80" t="s">
@@ -3163,14 +3186,14 @@
       <c r="W33" s="50"/>
     </row>
     <row r="34" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="54">
+      <c r="A34" s="78">
         <v>26</v>
       </c>
       <c r="B34" s="57" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C34" s="80">
-        <v>8420323</v>
+        <v>8426176</v>
       </c>
       <c r="D34" s="46" t="s">
         <v>65</v>
@@ -3180,6 +3203,9 @@
       </c>
       <c r="F34" s="85" t="s">
         <v>94</v>
+      </c>
+      <c r="G34" s="55" t="s">
+        <v>67</v>
       </c>
       <c r="H34" s="55"/>
       <c r="I34" s="55"/>
@@ -3190,11 +3216,13 @@
         <v>67</v>
       </c>
       <c r="N34" s="54"/>
-      <c r="O34" s="55"/>
+      <c r="O34" s="55" t="s">
+        <v>67</v>
+      </c>
       <c r="P34" s="55"/>
       <c r="Q34" s="55"/>
       <c r="R34" s="55" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S34" s="61"/>
       <c r="T34" s="80" t="s">
@@ -3207,23 +3235,23 @@
       <c r="W34" s="50"/>
     </row>
     <row r="35" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54">
+      <c r="A35" s="78">
         <v>27</v>
       </c>
       <c r="B35" s="57" t="s">
-        <v>198</v>
-      </c>
-      <c r="C35" s="55" t="s">
-        <v>155</v>
+        <v>246</v>
+      </c>
+      <c r="C35" s="80">
+        <v>8420323</v>
       </c>
       <c r="D35" s="46" t="s">
-        <v>144</v>
-      </c>
-      <c r="E35" s="55" t="s">
-        <v>150</v>
+        <v>65</v>
+      </c>
+      <c r="E35" s="80" t="s">
+        <v>93</v>
       </c>
       <c r="F35" s="85" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="G35" s="55" t="s">
         <v>67</v>
@@ -3233,17 +3261,21 @@
       <c r="J35" s="55"/>
       <c r="K35" s="55"/>
       <c r="L35" s="55"/>
-      <c r="M35" s="55"/>
-      <c r="N35" s="55"/>
+      <c r="M35" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="N35" s="54"/>
       <c r="O35" s="55" t="s">
         <v>67</v>
       </c>
       <c r="P35" s="55"/>
-      <c r="Q35" s="54"/>
-      <c r="R35" s="55"/>
+      <c r="Q35" s="55"/>
+      <c r="R35" s="55" t="s">
+        <v>243</v>
+      </c>
       <c r="S35" s="61"/>
       <c r="T35" s="80" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="U35" s="55" t="s">
         <v>67</v>
@@ -3252,20 +3284,20 @@
       <c r="W35" s="50"/>
     </row>
     <row r="36" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="54">
+      <c r="A36" s="78">
         <v>28</v>
       </c>
-      <c r="B36" s="86" t="s">
-        <v>199</v>
-      </c>
-      <c r="C36" s="86" t="s">
-        <v>156</v>
-      </c>
-      <c r="D36" s="87" t="s">
-        <v>145</v>
-      </c>
-      <c r="E36" s="86" t="s">
-        <v>153</v>
+      <c r="B36" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="C36" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" s="55" t="s">
+        <v>150</v>
       </c>
       <c r="F36" s="85" t="s">
         <v>54</v>
@@ -3297,20 +3329,20 @@
       <c r="W36" s="50"/>
     </row>
     <row r="37" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="54">
+      <c r="A37" s="78">
         <v>29</v>
       </c>
-      <c r="B37" s="55" t="s">
-        <v>200</v>
-      </c>
-      <c r="C37" s="55" t="s">
-        <v>157</v>
-      </c>
-      <c r="D37" s="54" t="s">
-        <v>146</v>
-      </c>
-      <c r="E37" s="55" t="s">
-        <v>151</v>
+      <c r="B37" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="C37" s="86" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="87" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="86" t="s">
+        <v>153</v>
       </c>
       <c r="F37" s="85" t="s">
         <v>54</v>
@@ -3320,9 +3352,7 @@
       </c>
       <c r="H37" s="55"/>
       <c r="I37" s="55"/>
-      <c r="J37" s="55" t="s">
-        <v>67</v>
-      </c>
+      <c r="J37" s="55"/>
       <c r="K37" s="55"/>
       <c r="L37" s="55"/>
       <c r="M37" s="55"/>
@@ -3331,33 +3361,33 @@
         <v>67</v>
       </c>
       <c r="P37" s="55"/>
-      <c r="Q37" s="83"/>
-      <c r="R37" s="83"/>
-      <c r="S37" s="83"/>
+      <c r="Q37" s="54"/>
+      <c r="R37" s="55"/>
+      <c r="S37" s="61"/>
       <c r="T37" s="80" t="s">
         <v>95</v>
       </c>
       <c r="U37" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="V37" s="83"/>
+      <c r="V37" s="55"/>
       <c r="W37" s="50"/>
     </row>
     <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="54">
+      <c r="A38" s="78">
         <v>30</v>
       </c>
-      <c r="B38" s="55" t="s">
-        <v>201</v>
+      <c r="B38" s="57" t="s">
+        <v>200</v>
       </c>
       <c r="C38" s="55" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D38" s="54" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F38" s="85" t="s">
         <v>54</v>
@@ -3367,7 +3397,9 @@
       </c>
       <c r="H38" s="55"/>
       <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
+      <c r="J38" s="55" t="s">
+        <v>67</v>
+      </c>
       <c r="K38" s="55"/>
       <c r="L38" s="55"/>
       <c r="M38" s="55"/>
@@ -3389,20 +3421,20 @@
       <c r="W38" s="50"/>
     </row>
     <row r="39" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54">
+      <c r="A39" s="78">
         <v>31</v>
       </c>
-      <c r="B39" s="55" t="s">
-        <v>202</v>
+      <c r="B39" s="57" t="s">
+        <v>201</v>
       </c>
       <c r="C39" s="55" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D39" s="54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F39" s="85" t="s">
         <v>54</v>
@@ -3413,9 +3445,7 @@
       <c r="H39" s="55"/>
       <c r="I39" s="55"/>
       <c r="J39" s="55"/>
-      <c r="K39" s="55" t="s">
-        <v>67</v>
-      </c>
+      <c r="K39" s="55"/>
       <c r="L39" s="55"/>
       <c r="M39" s="55"/>
       <c r="N39" s="55"/>
@@ -3436,14 +3466,14 @@
       <c r="W39" s="50"/>
     </row>
     <row r="40" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="54">
+      <c r="A40" s="78">
         <v>32</v>
       </c>
-      <c r="B40" s="55" t="s">
-        <v>203</v>
+      <c r="B40" s="57" t="s">
+        <v>202</v>
       </c>
       <c r="C40" s="55" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D40" s="54" t="s">
         <v>148</v>
@@ -3470,27 +3500,27 @@
         <v>67</v>
       </c>
       <c r="P40" s="55"/>
-      <c r="Q40" s="55"/>
-      <c r="R40" s="55"/>
-      <c r="S40" s="55"/>
+      <c r="Q40" s="83"/>
+      <c r="R40" s="83"/>
+      <c r="S40" s="83"/>
       <c r="T40" s="80" t="s">
         <v>95</v>
       </c>
       <c r="U40" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="V40" s="55"/>
+      <c r="V40" s="83"/>
       <c r="W40" s="50"/>
     </row>
     <row r="41" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="54">
+      <c r="A41" s="78">
         <v>33</v>
       </c>
-      <c r="B41" s="55" t="s">
-        <v>204</v>
+      <c r="B41" s="57" t="s">
+        <v>203</v>
       </c>
       <c r="C41" s="55" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D41" s="54" t="s">
         <v>148</v>
@@ -3530,14 +3560,14 @@
       <c r="W41" s="50"/>
     </row>
     <row r="42" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="54">
+      <c r="A42" s="78">
         <v>34</v>
       </c>
-      <c r="B42" s="55" t="s">
-        <v>205</v>
+      <c r="B42" s="57" t="s">
+        <v>204</v>
       </c>
       <c r="C42" s="55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D42" s="54" t="s">
         <v>148</v>
@@ -3574,16 +3604,17 @@
         <v>67</v>
       </c>
       <c r="V42" s="55"/>
+      <c r="W42" s="50"/>
     </row>
     <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="54">
+      <c r="A43" s="78">
         <v>35</v>
       </c>
-      <c r="B43" s="55" t="s">
-        <v>206</v>
+      <c r="B43" s="57" t="s">
+        <v>205</v>
       </c>
       <c r="C43" s="55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D43" s="54" t="s">
         <v>148</v>
@@ -3622,14 +3653,14 @@
       <c r="V43" s="55"/>
     </row>
     <row r="44" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="54">
+      <c r="A44" s="78">
         <v>36</v>
       </c>
-      <c r="B44" s="55" t="s">
-        <v>207</v>
+      <c r="B44" s="57" t="s">
+        <v>206</v>
       </c>
       <c r="C44" s="55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D44" s="54" t="s">
         <v>148</v>
@@ -3668,14 +3699,14 @@
       <c r="V44" s="55"/>
     </row>
     <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="54">
+      <c r="A45" s="78">
         <v>37</v>
       </c>
-      <c r="B45" s="55" t="s">
-        <v>208</v>
+      <c r="B45" s="57" t="s">
+        <v>207</v>
       </c>
       <c r="C45" s="55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D45" s="54" t="s">
         <v>148</v>
@@ -3714,14 +3745,14 @@
       <c r="V45" s="55"/>
     </row>
     <row r="46" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="54">
+      <c r="A46" s="78">
         <v>38</v>
       </c>
-      <c r="B46" s="55" t="s">
-        <v>209</v>
+      <c r="B46" s="57" t="s">
+        <v>208</v>
       </c>
       <c r="C46" s="55" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D46" s="54" t="s">
         <v>148</v>
@@ -3760,14 +3791,14 @@
       <c r="V46" s="55"/>
     </row>
     <row r="47" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="54">
+      <c r="A47" s="78">
         <v>39</v>
       </c>
-      <c r="B47" s="55" t="s">
-        <v>210</v>
+      <c r="B47" s="57" t="s">
+        <v>209</v>
       </c>
       <c r="C47" s="55" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D47" s="54" t="s">
         <v>148</v>
@@ -3806,14 +3837,14 @@
       <c r="V47" s="55"/>
     </row>
     <row r="48" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="54">
+      <c r="A48" s="78">
         <v>40</v>
       </c>
-      <c r="B48" s="55" t="s">
-        <v>211</v>
+      <c r="B48" s="57" t="s">
+        <v>210</v>
       </c>
       <c r="C48" s="55" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D48" s="54" t="s">
         <v>148</v>
@@ -3852,14 +3883,14 @@
       <c r="V48" s="55"/>
     </row>
     <row r="49" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="54">
+      <c r="A49" s="78">
         <v>41</v>
       </c>
-      <c r="B49" s="55" t="s">
-        <v>212</v>
+      <c r="B49" s="57" t="s">
+        <v>211</v>
       </c>
       <c r="C49" s="55" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D49" s="54" t="s">
         <v>148</v>
@@ -3898,14 +3929,14 @@
       <c r="V49" s="55"/>
     </row>
     <row r="50" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="54">
+      <c r="A50" s="78">
         <v>42</v>
       </c>
-      <c r="B50" s="55" t="s">
-        <v>213</v>
+      <c r="B50" s="57" t="s">
+        <v>212</v>
       </c>
       <c r="C50" s="55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D50" s="54" t="s">
         <v>148</v>
@@ -3944,14 +3975,14 @@
       <c r="V50" s="55"/>
     </row>
     <row r="51" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="54">
+      <c r="A51" s="78">
         <v>43</v>
       </c>
-      <c r="B51" s="55" t="s">
-        <v>214</v>
+      <c r="B51" s="57" t="s">
+        <v>213</v>
       </c>
       <c r="C51" s="55" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D51" s="54" t="s">
         <v>148</v>
@@ -3990,14 +4021,14 @@
       <c r="V51" s="55"/>
     </row>
     <row r="52" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="54">
+      <c r="A52" s="78">
         <v>44</v>
       </c>
-      <c r="B52" s="55" t="s">
-        <v>215</v>
+      <c r="B52" s="57" t="s">
+        <v>214</v>
       </c>
       <c r="C52" s="55" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D52" s="54" t="s">
         <v>148</v>
@@ -4036,14 +4067,14 @@
       <c r="V52" s="55"/>
     </row>
     <row r="53" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="54">
+      <c r="A53" s="78">
         <v>45</v>
       </c>
-      <c r="B53" s="55" t="s">
-        <v>216</v>
+      <c r="B53" s="57" t="s">
+        <v>215</v>
       </c>
       <c r="C53" s="55" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D53" s="54" t="s">
         <v>148</v>
@@ -4082,14 +4113,14 @@
       <c r="V53" s="55"/>
     </row>
     <row r="54" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="54">
+      <c r="A54" s="78">
         <v>46</v>
       </c>
-      <c r="B54" s="55" t="s">
-        <v>217</v>
+      <c r="B54" s="57" t="s">
+        <v>216</v>
       </c>
       <c r="C54" s="55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D54" s="54" t="s">
         <v>148</v>
@@ -4128,14 +4159,14 @@
       <c r="V54" s="55"/>
     </row>
     <row r="55" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="54">
+      <c r="A55" s="78">
         <v>47</v>
       </c>
-      <c r="B55" s="55" t="s">
-        <v>218</v>
+      <c r="B55" s="57" t="s">
+        <v>217</v>
       </c>
       <c r="C55" s="55" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D55" s="54" t="s">
         <v>148</v>
@@ -4174,14 +4205,14 @@
       <c r="V55" s="55"/>
     </row>
     <row r="56" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="54">
+      <c r="A56" s="78">
         <v>48</v>
       </c>
-      <c r="B56" s="55" t="s">
-        <v>219</v>
+      <c r="B56" s="57" t="s">
+        <v>218</v>
       </c>
       <c r="C56" s="55" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D56" s="54" t="s">
         <v>148</v>
@@ -4220,14 +4251,14 @@
       <c r="V56" s="55"/>
     </row>
     <row r="57" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="54">
+      <c r="A57" s="78">
         <v>49</v>
       </c>
-      <c r="B57" s="55" t="s">
-        <v>220</v>
+      <c r="B57" s="57" t="s">
+        <v>219</v>
       </c>
       <c r="C57" s="55" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D57" s="54" t="s">
         <v>148</v>
@@ -4266,14 +4297,14 @@
       <c r="V57" s="55"/>
     </row>
     <row r="58" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="54">
+      <c r="A58" s="78">
         <v>50</v>
       </c>
-      <c r="B58" s="55" t="s">
-        <v>221</v>
+      <c r="B58" s="57" t="s">
+        <v>220</v>
       </c>
       <c r="C58" s="55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D58" s="54" t="s">
         <v>148</v>
@@ -4312,14 +4343,14 @@
       <c r="V58" s="55"/>
     </row>
     <row r="59" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="54">
+      <c r="A59" s="78">
         <v>51</v>
       </c>
-      <c r="B59" s="55" t="s">
-        <v>222</v>
+      <c r="B59" s="57" t="s">
+        <v>221</v>
       </c>
       <c r="C59" s="55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D59" s="54" t="s">
         <v>148</v>
@@ -4358,14 +4389,14 @@
       <c r="V59" s="55"/>
     </row>
     <row r="60" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="54">
+      <c r="A60" s="78">
         <v>52</v>
       </c>
-      <c r="B60" s="55" t="s">
-        <v>223</v>
+      <c r="B60" s="57" t="s">
+        <v>222</v>
       </c>
       <c r="C60" s="55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D60" s="54" t="s">
         <v>148</v>
@@ -4404,17 +4435,17 @@
       <c r="V60" s="55"/>
     </row>
     <row r="61" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="54">
+      <c r="A61" s="78">
         <v>53</v>
       </c>
-      <c r="B61" s="55" t="s">
-        <v>224</v>
+      <c r="B61" s="57" t="s">
+        <v>223</v>
       </c>
       <c r="C61" s="55" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D61" s="54" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E61" s="55" t="s">
         <v>154</v>
@@ -4428,10 +4459,10 @@
       <c r="H61" s="55"/>
       <c r="I61" s="55"/>
       <c r="J61" s="55"/>
-      <c r="K61" s="55"/>
-      <c r="L61" s="55" t="s">
-        <v>67</v>
-      </c>
+      <c r="K61" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="L61" s="55"/>
       <c r="M61" s="55"/>
       <c r="N61" s="55"/>
       <c r="O61" s="55" t="s">
@@ -4450,14 +4481,14 @@
       <c r="V61" s="55"/>
     </row>
     <row r="62" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="54">
+      <c r="A62" s="78">
         <v>54</v>
       </c>
-      <c r="B62" s="55" t="s">
-        <v>225</v>
+      <c r="B62" s="57" t="s">
+        <v>224</v>
       </c>
       <c r="C62" s="55" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D62" s="54" t="s">
         <v>149</v>
@@ -4496,14 +4527,14 @@
       <c r="V62" s="55"/>
     </row>
     <row r="63" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="54">
+      <c r="A63" s="78">
         <v>55</v>
       </c>
-      <c r="B63" s="55" t="s">
-        <v>226</v>
+      <c r="B63" s="57" t="s">
+        <v>225</v>
       </c>
       <c r="C63" s="55" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D63" s="54" t="s">
         <v>149</v>
@@ -4542,14 +4573,14 @@
       <c r="V63" s="55"/>
     </row>
     <row r="64" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="54">
+      <c r="A64" s="78">
         <v>56</v>
       </c>
-      <c r="B64" s="55" t="s">
-        <v>227</v>
+      <c r="B64" s="57" t="s">
+        <v>226</v>
       </c>
       <c r="C64" s="55" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D64" s="54" t="s">
         <v>149</v>
@@ -4588,14 +4619,14 @@
       <c r="V64" s="55"/>
     </row>
     <row r="65" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="54">
+      <c r="A65" s="78">
         <v>57</v>
       </c>
-      <c r="B65" s="55" t="s">
-        <v>228</v>
+      <c r="B65" s="57" t="s">
+        <v>227</v>
       </c>
       <c r="C65" s="55" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D65" s="54" t="s">
         <v>149</v>
@@ -4634,14 +4665,14 @@
       <c r="V65" s="55"/>
     </row>
     <row r="66" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="54">
+      <c r="A66" s="78">
         <v>58</v>
       </c>
-      <c r="B66" s="55" t="s">
-        <v>229</v>
+      <c r="B66" s="57" t="s">
+        <v>228</v>
       </c>
       <c r="C66" s="55" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D66" s="54" t="s">
         <v>149</v>
@@ -4680,14 +4711,14 @@
       <c r="V66" s="55"/>
     </row>
     <row r="67" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="54">
+      <c r="A67" s="78">
         <v>59</v>
       </c>
-      <c r="B67" s="55" t="s">
-        <v>230</v>
+      <c r="B67" s="57" t="s">
+        <v>229</v>
       </c>
       <c r="C67" s="55" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D67" s="54" t="s">
         <v>149</v>
@@ -4726,14 +4757,14 @@
       <c r="V67" s="55"/>
     </row>
     <row r="68" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="54">
+      <c r="A68" s="78">
         <v>60</v>
       </c>
-      <c r="B68" s="55" t="s">
-        <v>231</v>
+      <c r="B68" s="57" t="s">
+        <v>230</v>
       </c>
       <c r="C68" s="55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D68" s="54" t="s">
         <v>149</v>
@@ -4772,14 +4803,14 @@
       <c r="V68" s="55"/>
     </row>
     <row r="69" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="54">
+      <c r="A69" s="78">
         <v>61</v>
       </c>
-      <c r="B69" s="55" t="s">
-        <v>232</v>
+      <c r="B69" s="57" t="s">
+        <v>231</v>
       </c>
       <c r="C69" s="55" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D69" s="54" t="s">
         <v>149</v>
@@ -4818,14 +4849,14 @@
       <c r="V69" s="55"/>
     </row>
     <row r="70" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="54">
+      <c r="A70" s="78">
         <v>62</v>
       </c>
-      <c r="B70" s="55" t="s">
-        <v>233</v>
+      <c r="B70" s="57" t="s">
+        <v>232</v>
       </c>
       <c r="C70" s="55" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D70" s="54" t="s">
         <v>149</v>
@@ -4864,14 +4895,14 @@
       <c r="V70" s="55"/>
     </row>
     <row r="71" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="54">
+      <c r="A71" s="78">
         <v>63</v>
       </c>
-      <c r="B71" s="55" t="s">
-        <v>234</v>
+      <c r="B71" s="57" t="s">
+        <v>233</v>
       </c>
       <c r="C71" s="55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D71" s="54" t="s">
         <v>149</v>
@@ -4898,7 +4929,7 @@
         <v>67</v>
       </c>
       <c r="P71" s="55"/>
-      <c r="Q71" s="54"/>
+      <c r="Q71" s="55"/>
       <c r="R71" s="55"/>
       <c r="S71" s="55"/>
       <c r="T71" s="80" t="s">
@@ -4910,14 +4941,14 @@
       <c r="V71" s="55"/>
     </row>
     <row r="72" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="54">
+      <c r="A72" s="78">
         <v>64</v>
       </c>
-      <c r="B72" s="55" t="s">
-        <v>235</v>
+      <c r="B72" s="57" t="s">
+        <v>234</v>
       </c>
       <c r="C72" s="55" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D72" s="54" t="s">
         <v>149</v>
@@ -4956,14 +4987,14 @@
       <c r="V72" s="55"/>
     </row>
     <row r="73" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="54">
+      <c r="A73" s="78">
         <v>65</v>
       </c>
-      <c r="B73" s="55" t="s">
-        <v>236</v>
+      <c r="B73" s="57" t="s">
+        <v>235</v>
       </c>
       <c r="C73" s="55" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D73" s="54" t="s">
         <v>149</v>
@@ -4971,7 +5002,7 @@
       <c r="E73" s="55" t="s">
         <v>154</v>
       </c>
-      <c r="F73" s="55" t="s">
+      <c r="F73" s="85" t="s">
         <v>54</v>
       </c>
       <c r="G73" s="55" t="s">
@@ -4993,7 +5024,7 @@
       <c r="Q73" s="54"/>
       <c r="R73" s="55"/>
       <c r="S73" s="55"/>
-      <c r="T73" s="55" t="s">
+      <c r="T73" s="80" t="s">
         <v>95</v>
       </c>
       <c r="U73" s="55" t="s">
@@ -5002,16 +5033,16 @@
       <c r="V73" s="55"/>
     </row>
     <row r="74" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="54">
+      <c r="A74" s="78">
         <v>66</v>
       </c>
-      <c r="B74" s="55" t="s">
-        <v>237</v>
+      <c r="B74" s="57" t="s">
+        <v>236</v>
       </c>
       <c r="C74" s="55" t="s">
-        <v>194</v>
-      </c>
-      <c r="D74" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="D74" s="54" t="s">
         <v>149</v>
       </c>
       <c r="E74" s="55" t="s">
@@ -5036,7 +5067,7 @@
         <v>67</v>
       </c>
       <c r="P74" s="55"/>
-      <c r="Q74" s="55"/>
+      <c r="Q74" s="54"/>
       <c r="R74" s="55"/>
       <c r="S74" s="55"/>
       <c r="T74" s="55" t="s">
@@ -5048,14 +5079,14 @@
       <c r="V74" s="55"/>
     </row>
     <row r="75" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="54">
-        <v>67</v>
-      </c>
-      <c r="B75" s="55" t="s">
-        <v>238</v>
+      <c r="A75" s="78">
+        <v>67</v>
+      </c>
+      <c r="B75" s="57" t="s">
+        <v>237</v>
       </c>
       <c r="C75" s="55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D75" s="55" t="s">
         <v>149</v>
@@ -5094,14 +5125,14 @@
       <c r="V75" s="55"/>
     </row>
     <row r="76" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="54">
+      <c r="A76" s="78">
         <v>68</v>
       </c>
-      <c r="B76" s="55" t="s">
-        <v>239</v>
+      <c r="B76" s="57" t="s">
+        <v>238</v>
       </c>
       <c r="C76" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D76" s="55" t="s">
         <v>149</v>
@@ -5140,14 +5171,14 @@
       <c r="V76" s="55"/>
     </row>
     <row r="77" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="54">
+      <c r="A77" s="78">
         <v>69</v>
       </c>
-      <c r="B77" s="55" t="s">
-        <v>240</v>
+      <c r="B77" s="57" t="s">
+        <v>239</v>
       </c>
       <c r="C77" s="55" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D77" s="55" t="s">
         <v>149</v>
@@ -5186,44 +5217,84 @@
       <c r="V77" s="55"/>
     </row>
     <row r="78" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D78" s="2"/>
+      <c r="A78" s="78">
+        <v>70</v>
+      </c>
+      <c r="B78" s="57" t="s">
+        <v>240</v>
+      </c>
+      <c r="C78" s="55" t="s">
+        <v>197</v>
+      </c>
+      <c r="D78" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E78" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="F78" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="G78" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="H78" s="55"/>
+      <c r="I78" s="55"/>
+      <c r="J78" s="55"/>
+      <c r="K78" s="55"/>
+      <c r="L78" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="M78" s="55"/>
+      <c r="N78" s="55"/>
+      <c r="O78" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="P78" s="55"/>
+      <c r="Q78" s="55"/>
+      <c r="R78" s="55"/>
+      <c r="S78" s="55"/>
+      <c r="T78" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="U78" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="V78" s="55"/>
     </row>
     <row r="79" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D80" s="2"/>
-      <c r="P80" s="92" t="s">
-        <v>247</v>
-      </c>
-      <c r="Q80" s="92"/>
-      <c r="R80" s="92"/>
-      <c r="S80" s="92"/>
-      <c r="T80" s="92"/>
-      <c r="U80" s="92"/>
     </row>
     <row r="81" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D81" s="2"/>
-      <c r="P81" s="99" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q81" s="99"/>
-      <c r="R81" s="99"/>
-      <c r="S81" s="99"/>
-      <c r="T81" s="99"/>
-      <c r="U81" s="99"/>
+      <c r="P81" s="94" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q81" s="94"/>
+      <c r="R81" s="94"/>
+      <c r="S81" s="94"/>
+      <c r="T81" s="94"/>
+      <c r="U81" s="94"/>
     </row>
     <row r="82" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D82" s="2"/>
-      <c r="S82" s="76"/>
-      <c r="T82" s="76"/>
-      <c r="U82" s="76"/>
+      <c r="P82" s="101" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q82" s="101"/>
+      <c r="R82" s="101"/>
+      <c r="S82" s="101"/>
+      <c r="T82" s="101"/>
+      <c r="U82" s="101"/>
     </row>
     <row r="83" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D83" s="2"/>
+      <c r="S83" s="76"/>
       <c r="T83" s="76"/>
       <c r="U83" s="76"/>
-      <c r="V83" s="76"/>
     </row>
     <row r="84" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D84" s="2"/>
@@ -5233,41 +5304,43 @@
     </row>
     <row r="85" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D85" s="2"/>
-      <c r="Q85" s="50"/>
-      <c r="R85" s="50"/>
+      <c r="T85" s="76"/>
+      <c r="U85" s="76"/>
+      <c r="V85" s="76"/>
     </row>
     <row r="86" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D86" s="2"/>
+      <c r="Q86" s="50"/>
+      <c r="R86" s="50"/>
     </row>
     <row r="87" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D87" s="2"/>
-      <c r="S87" s="77"/>
     </row>
     <row r="88" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D88" s="2"/>
-      <c r="Q88" s="91"/>
-      <c r="R88" s="91"/>
-      <c r="T88" s="92" t="s">
-        <v>47</v>
-      </c>
-      <c r="U88" s="92"/>
-      <c r="V88" s="92"/>
+      <c r="S88" s="77"/>
     </row>
     <row r="89" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D89" s="2"/>
-      <c r="Q89" s="93" t="s">
-        <v>45</v>
-      </c>
+      <c r="Q89" s="93"/>
       <c r="R89" s="93"/>
-      <c r="T89" s="92" t="s">
-        <v>46</v>
-      </c>
-      <c r="U89" s="92"/>
-      <c r="V89" s="92"/>
+      <c r="T89" s="94" t="s">
+        <v>47</v>
+      </c>
+      <c r="U89" s="94"/>
+      <c r="V89" s="94"/>
     </row>
     <row r="90" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D90" s="2"/>
-      <c r="Q90" s="3"/>
+      <c r="Q90" s="95" t="s">
+        <v>45</v>
+      </c>
+      <c r="R90" s="95"/>
+      <c r="T90" s="94" t="s">
+        <v>46</v>
+      </c>
+      <c r="U90" s="94"/>
+      <c r="V90" s="94"/>
     </row>
     <row r="91" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D91" s="2"/>
@@ -5287,6 +5360,7 @@
     </row>
     <row r="95" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D95" s="2"/>
+      <c r="Q95" s="3"/>
     </row>
     <row r="96" spans="4:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D96" s="2"/>
@@ -5317,7 +5391,6 @@
     </row>
     <row r="105" spans="4:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
-      <c r="Q105" s="3"/>
     </row>
     <row r="106" spans="4:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D106" s="2"/>
@@ -8911,20 +8984,24 @@
       <c r="D1003" s="2"/>
       <c r="Q1003" s="3"/>
     </row>
+    <row r="1004" spans="4:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1004" s="2"/>
+      <c r="Q1004" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="Q88:R88"/>
-    <mergeCell ref="T88:V88"/>
     <mergeCell ref="Q89:R89"/>
     <mergeCell ref="T89:V89"/>
+    <mergeCell ref="Q90:R90"/>
+    <mergeCell ref="T90:V90"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="U7:V7"/>
-    <mergeCell ref="P80:U80"/>
     <mergeCell ref="P81:U81"/>
+    <mergeCell ref="P82:U82"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="50" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="49" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8963,28 +9040,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="95"/>
-      <c r="S1" s="95"/>
-      <c r="T1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="97"/>
+      <c r="S1" s="97"/>
+      <c r="T1" s="98"/>
     </row>
     <row r="2" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -9092,10 +9169,10 @@
       <c r="T7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="U7" s="97" t="s">
+      <c r="U7" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="V7" s="98"/>
+      <c r="V7" s="100"/>
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
@@ -12278,19 +12355,19 @@
     </row>
     <row r="128" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D128" s="2"/>
-      <c r="Q128" s="100" t="s">
+      <c r="Q128" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="R128" s="101"/>
-      <c r="S128" s="101"/>
+      <c r="R128" s="103"/>
+      <c r="S128" s="103"/>
     </row>
     <row r="129" spans="4:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D129" s="2"/>
-      <c r="Q129" s="102" t="s">
+      <c r="Q129" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="R129" s="101"/>
-      <c r="S129" s="101"/>
+      <c r="R129" s="103"/>
+      <c r="S129" s="103"/>
     </row>
     <row r="130" spans="4:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D130" s="2"/>

</xml_diff>